<commit_message>
Add 6th exercise AVD1 files
</commit_message>
<xml_diff>
--- a/AVD1/5 - Ondřej Švorc - Retence.xlsx
+++ b/AVD1/5 - Ondřej Švorc - Retence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UJEP\AVD1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EB69BC-71AD-4CE3-873C-C6EA64E358C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE8760F-79D0-455D-B1F1-E5D9ECC76D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3095BA0B-7F52-4A9A-9669-92A26B1E4A80}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="208">
   <si>
     <t>ID GAMA</t>
   </si>
@@ -546,9 +546,6 @@
     <t>2.1.2023</t>
   </si>
   <si>
-    <t>Nedovoláno</t>
-  </si>
-  <si>
     <t>5.1.2023</t>
   </si>
   <si>
@@ -561,9 +558,6 @@
     <t>zůstává s premií</t>
   </si>
   <si>
-    <t>Zůstává s prémií</t>
-  </si>
-  <si>
     <t>pom</t>
   </si>
   <si>
@@ -619,12 +613,69 @@
   </si>
   <si>
     <t>Normálně platí 200 Kč, ale prvních 6 měsíců mu prostě posíláme 350 Kč, takže jako je v plusu 150 Kč klient</t>
+  </si>
+  <si>
+    <t>nedovoláno:</t>
+  </si>
+  <si>
+    <t>náklad za přijatý hovor:</t>
+  </si>
+  <si>
+    <t>náklad za nepřijatý hovor:</t>
+  </si>
+  <si>
+    <t>přechod k jinému poskytovateli:</t>
+  </si>
+  <si>
+    <t>rozmýšlí si:</t>
+  </si>
+  <si>
+    <t>zůstává s premií:</t>
+  </si>
+  <si>
+    <t>náklad</t>
+  </si>
+  <si>
+    <t>počet</t>
+  </si>
+  <si>
+    <t>celkové náklady:</t>
+  </si>
+  <si>
+    <t>fakta:</t>
+  </si>
+  <si>
+    <t>sleva 350 Kč/měsíc na 6 měsíců při prodloužení smlouvy o 18 měsíců (aplikujeme momentálně pouze na ty, co zůstávají s prémií)</t>
+  </si>
+  <si>
+    <t>každý klient co má u vaší společnosti smlouvu, generuje průměrný výnos 200 Kč měsíčně</t>
+  </si>
+  <si>
+    <t>18 měsíců přináší 200 Kč/měsíčně</t>
+  </si>
+  <si>
+    <t>Zároveň mu ale dáváme slevu 350 Kč/měsíčně po dobu 6 měsíců</t>
+  </si>
+  <si>
+    <t>Tedy po odečtení, čistý výnos z klienta, který zůstane bude za 18 měsíců</t>
+  </si>
+  <si>
+    <t>Čistý výnos z klientů, kteří zůstanou bude za 18 měsíců:</t>
+  </si>
+  <si>
+    <t>Čistý výnos retenční kampaně:</t>
+  </si>
+  <si>
+    <t>Poměr návratnosti (ROI):</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#,##0\ &quot;Kč&quot;"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,7 +703,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -660,13 +711,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1307,64 +1393,64 @@
   </sheetPr>
   <dimension ref="A24:M33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1378,7 +1464,7 @@
   <dimension ref="A1:C151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3060,7 +3146,7 @@
   <dimension ref="B3:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,7 +3168,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -3098,7 +3184,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -3106,7 +3192,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -3114,7 +3200,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -3122,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3132,10 +3218,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020EC039-F7E7-4DEF-AE9A-E6C4DE324E37}">
-  <dimension ref="B2:F158"/>
+  <dimension ref="B2:R158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3143,9 +3229,13 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>160</v>
       </c>
@@ -3155,8 +3245,15 @@
       <c r="D2" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N2" s="5"/>
+      <c r="O2" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -3167,10 +3264,21 @@
         <v>164</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="O3" s="5">
+        <f>COUNTIF($C$3:$C$158, "nedovoláno")</f>
+        <v>69</v>
+      </c>
+      <c r="P3" s="8">
+        <f>O3*$O$9</f>
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>66</v>
       </c>
@@ -3180,8 +3288,19 @@
       <c r="D4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N4" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="O4" s="5">
+        <f>COUNTIF($C$3:$C$158, "přechod k jinému poskytovateli")</f>
+        <v>27</v>
+      </c>
+      <c r="P4" s="8">
+        <f>O4*$O$8</f>
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>67</v>
       </c>
@@ -3191,8 +3310,19 @@
       <c r="D5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N5" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="O5" s="5">
+        <f>COUNTIF($C$3:$C$158, "rozmýšlí si")</f>
+        <v>11</v>
+      </c>
+      <c r="P5" s="8">
+        <f>O5*$O$8</f>
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>68</v>
       </c>
@@ -3202,8 +3332,19 @@
       <c r="D6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N6" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="O6" s="5">
+        <f>COUNTIF($C$3:$C$158, "zůstává s premií")</f>
+        <v>49</v>
+      </c>
+      <c r="P6" s="8">
+        <f>O6*$O$8</f>
+        <v>4655</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>69</v>
       </c>
@@ -3213,8 +3354,9 @@
       <c r="D7" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>72</v>
       </c>
@@ -3224,8 +3366,14 @@
       <c r="D8" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="O8" s="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -3235,19 +3383,25 @@
       <c r="D9" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N9" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="O9" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -3257,8 +3411,15 @@
       <c r="D11" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N11" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="O11" s="3">
+        <f>SUM(P3:P6)</f>
+        <v>10680</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>122</v>
       </c>
@@ -3268,8 +3429,10 @@
       <c r="D12" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N12" s="9"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>73</v>
       </c>
@@ -3280,7 +3443,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -3288,10 +3451,10 @@
         <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>74</v>
       </c>
@@ -3301,8 +3464,11 @@
       <c r="D15" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>75</v>
       </c>
@@ -3312,8 +3478,11 @@
       <c r="D16" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>76</v>
       </c>
@@ -3323,8 +3492,11 @@
       <c r="D17" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -3335,7 +3507,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>77</v>
       </c>
@@ -3345,8 +3517,15 @@
       <c r="D19" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>202</v>
+      </c>
+      <c r="R19" s="3">
+        <f>18*200</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>78</v>
       </c>
@@ -3356,8 +3535,15 @@
       <c r="D20" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>203</v>
+      </c>
+      <c r="R20" s="3">
+        <f>6*350</f>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -3365,10 +3551,17 @@
         <v>163</v>
       </c>
       <c r="D21" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="N21" t="s">
+        <v>204</v>
+      </c>
+      <c r="R21" s="3">
+        <f>R19-R20</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>79</v>
       </c>
@@ -3378,8 +3571,15 @@
       <c r="D22" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>205</v>
+      </c>
+      <c r="R22" s="3">
+        <f>49*R21</f>
+        <v>73500</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>80</v>
       </c>
@@ -3389,19 +3589,33 @@
       <c r="D23" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N23" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="R23" s="3">
+        <f>R22-O11</f>
+        <v>62820</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D24" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>207</v>
+      </c>
+      <c r="R24" s="11">
+        <f>R23 / O11</f>
+        <v>5.882022471910112</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>82</v>
       </c>
@@ -3409,10 +3623,10 @@
         <v>163</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>83</v>
       </c>
@@ -3423,7 +3637,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>84</v>
       </c>
@@ -3433,8 +3647,12 @@
       <c r="D27" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <f>(27)*200</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>13</v>
       </c>
@@ -3444,8 +3662,12 @@
       <c r="D28" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <f>11*200</f>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -3455,8 +3677,12 @@
       <c r="D29" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <f>69*200</f>
+        <v>13800</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -3467,23 +3693,23 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D31" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D32" t="s">
         <v>165</v>
@@ -3530,7 +3756,7 @@
         <v>163</v>
       </c>
       <c r="D36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -3563,7 +3789,7 @@
         <v>163</v>
       </c>
       <c r="D39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -3637,7 +3863,7 @@
         <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D46" t="s">
         <v>165</v>
@@ -3651,7 +3877,7 @@
         <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
@@ -3681,7 +3907,7 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D50" t="s">
         <v>165</v>
@@ -3714,7 +3940,7 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D53" t="s">
         <v>165</v>
@@ -3838,7 +4064,7 @@
         <v>163</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
@@ -3923,7 +4149,7 @@
         <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D72" t="s">
         <v>165</v>
@@ -3934,10 +4160,10 @@
         <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
@@ -3945,7 +4171,7 @@
         <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D74" t="s">
         <v>164</v>
@@ -3956,7 +4182,7 @@
         <v>97</v>
       </c>
       <c r="C75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D75" t="s">
         <v>165</v>
@@ -3967,7 +4193,7 @@
         <v>85</v>
       </c>
       <c r="C76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D76" t="s">
         <v>165</v>
@@ -3978,7 +4204,7 @@
         <v>86</v>
       </c>
       <c r="C77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D77" t="s">
         <v>165</v>
@@ -3989,7 +4215,7 @@
         <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D78" t="s">
         <v>165</v>
@@ -4000,7 +4226,7 @@
         <v>87</v>
       </c>
       <c r="C79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D79" t="s">
         <v>165</v>
@@ -4011,7 +4237,7 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D80" t="s">
         <v>165</v>
@@ -4022,7 +4248,7 @@
         <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D81" t="s">
         <v>165</v>
@@ -4033,7 +4259,7 @@
         <v>102</v>
       </c>
       <c r="C82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D82" t="s">
         <v>165</v>
@@ -4044,7 +4270,7 @@
         <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D83" t="s">
         <v>165</v>
@@ -4055,7 +4281,7 @@
         <v>88</v>
       </c>
       <c r="C84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D84" t="s">
         <v>165</v>
@@ -4066,7 +4292,7 @@
         <v>104</v>
       </c>
       <c r="C85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D85" t="s">
         <v>165</v>
@@ -4077,7 +4303,7 @@
         <v>89</v>
       </c>
       <c r="C86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D86" t="s">
         <v>165</v>
@@ -4088,7 +4314,7 @@
         <v>105</v>
       </c>
       <c r="C87" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D87" t="s">
         <v>165</v>
@@ -4099,7 +4325,7 @@
         <v>106</v>
       </c>
       <c r="C88" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D88" t="s">
         <v>165</v>
@@ -4110,10 +4336,10 @@
         <v>90</v>
       </c>
       <c r="C89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
@@ -4121,7 +4347,7 @@
         <v>107</v>
       </c>
       <c r="C90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D90" t="s">
         <v>165</v>
@@ -4132,10 +4358,10 @@
         <v>91</v>
       </c>
       <c r="C91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
@@ -4143,7 +4369,7 @@
         <v>108</v>
       </c>
       <c r="C92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D92" t="s">
         <v>165</v>
@@ -4154,7 +4380,7 @@
         <v>96</v>
       </c>
       <c r="C93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D93" t="s">
         <v>165</v>
@@ -4165,7 +4391,7 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D94" t="s">
         <v>165</v>
@@ -4176,7 +4402,7 @@
         <v>109</v>
       </c>
       <c r="C95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D95" t="s">
         <v>166</v>
@@ -4187,7 +4413,7 @@
         <v>110</v>
       </c>
       <c r="C96" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D96" t="s">
         <v>165</v>
@@ -4198,7 +4424,7 @@
         <v>15</v>
       </c>
       <c r="C97" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D97" t="s">
         <v>165</v>
@@ -4209,7 +4435,7 @@
         <v>111</v>
       </c>
       <c r="C98" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D98" t="s">
         <v>164</v>
@@ -4220,7 +4446,7 @@
         <v>116</v>
       </c>
       <c r="C99" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D99" t="s">
         <v>165</v>
@@ -4231,7 +4457,7 @@
         <v>117</v>
       </c>
       <c r="C100" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D100" t="s">
         <v>166</v>
@@ -4242,10 +4468,10 @@
         <v>123</v>
       </c>
       <c r="C101" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D101" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
@@ -4253,10 +4479,10 @@
         <v>118</v>
       </c>
       <c r="C102" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D102" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
@@ -4264,7 +4490,7 @@
         <v>119</v>
       </c>
       <c r="C103" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D103" t="s">
         <v>165</v>
@@ -4275,10 +4501,10 @@
         <v>120</v>
       </c>
       <c r="C104" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
@@ -4286,7 +4512,7 @@
         <v>124</v>
       </c>
       <c r="C105" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D105" t="s">
         <v>165</v>
@@ -4297,7 +4523,7 @@
         <v>125</v>
       </c>
       <c r="C106" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D106" t="s">
         <v>165</v>
@@ -4308,7 +4534,7 @@
         <v>114</v>
       </c>
       <c r="C107" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D107" t="s">
         <v>165</v>
@@ -4319,7 +4545,7 @@
         <v>121</v>
       </c>
       <c r="C108" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D108" t="s">
         <v>165</v>
@@ -4330,10 +4556,10 @@
         <v>115</v>
       </c>
       <c r="C109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
@@ -4341,10 +4567,10 @@
         <v>122</v>
       </c>
       <c r="C110" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
@@ -4352,7 +4578,7 @@
         <v>123</v>
       </c>
       <c r="C111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D111" t="s">
         <v>165</v>
@@ -4363,7 +4589,7 @@
         <v>129</v>
       </c>
       <c r="C112" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D112" t="s">
         <v>165</v>
@@ -4374,7 +4600,7 @@
         <v>149</v>
       </c>
       <c r="C113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D113" t="s">
         <v>165</v>
@@ -4385,7 +4611,7 @@
         <v>143</v>
       </c>
       <c r="C114" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D114" t="s">
         <v>165</v>
@@ -4396,7 +4622,7 @@
         <v>136</v>
       </c>
       <c r="C115" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D115" t="s">
         <v>165</v>
@@ -4407,7 +4633,7 @@
         <v>151</v>
       </c>
       <c r="C116" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D116" t="s">
         <v>165</v>
@@ -4418,7 +4644,7 @@
         <v>152</v>
       </c>
       <c r="C117" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D117" t="s">
         <v>165</v>
@@ -4429,7 +4655,7 @@
         <v>70</v>
       </c>
       <c r="C118" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D118" t="s">
         <v>165</v>
@@ -4440,7 +4666,7 @@
         <v>146</v>
       </c>
       <c r="C119" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D119" t="s">
         <v>166</v>
@@ -4451,7 +4677,7 @@
         <v>71</v>
       </c>
       <c r="C120" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D120" t="s">
         <v>165</v>
@@ -4462,7 +4688,7 @@
         <v>153</v>
       </c>
       <c r="C121" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D121" t="s">
         <v>165</v>
@@ -4473,10 +4699,10 @@
         <v>154</v>
       </c>
       <c r="C122" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D122" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
@@ -4484,7 +4710,7 @@
         <v>137</v>
       </c>
       <c r="C123" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D123" t="s">
         <v>165</v>
@@ -4495,10 +4721,10 @@
         <v>138</v>
       </c>
       <c r="C124" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D124" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4732,7 @@
         <v>139</v>
       </c>
       <c r="C125" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D125" t="s">
         <v>165</v>
@@ -4517,7 +4743,7 @@
         <v>155</v>
       </c>
       <c r="C126" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D126" t="s">
         <v>164</v>
@@ -4528,7 +4754,7 @@
         <v>156</v>
       </c>
       <c r="C127" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D127" t="s">
         <v>165</v>
@@ -4539,7 +4765,7 @@
         <v>140</v>
       </c>
       <c r="C128" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D128" t="s">
         <v>164</v>
@@ -4550,7 +4776,7 @@
         <v>141</v>
       </c>
       <c r="C129" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D129" t="s">
         <v>165</v>
@@ -4561,10 +4787,10 @@
         <v>157</v>
       </c>
       <c r="C130" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D130" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
@@ -4572,7 +4798,7 @@
         <v>142</v>
       </c>
       <c r="C131" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D131" t="s">
         <v>165</v>
@@ -4583,10 +4809,10 @@
         <v>147</v>
       </c>
       <c r="C132" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D132" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
@@ -4594,7 +4820,7 @@
         <v>148</v>
       </c>
       <c r="C133" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D133" t="s">
         <v>165</v>
@@ -4605,7 +4831,7 @@
         <v>16</v>
       </c>
       <c r="C134" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D134" t="s">
         <v>164</v>
@@ -4616,7 +4842,7 @@
         <v>28</v>
       </c>
       <c r="C135" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D135" t="s">
         <v>165</v>
@@ -4627,7 +4853,7 @@
         <v>128</v>
       </c>
       <c r="C136" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D136" t="s">
         <v>165</v>
@@ -4638,7 +4864,7 @@
         <v>30</v>
       </c>
       <c r="C137" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D137" t="s">
         <v>166</v>
@@ -4649,7 +4875,7 @@
         <v>100</v>
       </c>
       <c r="C138" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D138" t="s">
         <v>165</v>
@@ -4660,7 +4886,7 @@
         <v>101</v>
       </c>
       <c r="C139" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D139" t="s">
         <v>165</v>
@@ -4671,7 +4897,7 @@
         <v>144</v>
       </c>
       <c r="C140" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D140" t="s">
         <v>165</v>
@@ -4682,10 +4908,10 @@
         <v>121</v>
       </c>
       <c r="C141" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D141" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
@@ -4693,10 +4919,10 @@
         <v>18</v>
       </c>
       <c r="C142" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D142" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
@@ -4704,7 +4930,7 @@
         <v>130</v>
       </c>
       <c r="C143" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D143" t="s">
         <v>165</v>
@@ -4715,7 +4941,7 @@
         <v>126</v>
       </c>
       <c r="C144" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D144" t="s">
         <v>165</v>
@@ -4726,7 +4952,7 @@
         <v>131</v>
       </c>
       <c r="C145" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D145" t="s">
         <v>165</v>
@@ -4737,7 +4963,7 @@
         <v>132</v>
       </c>
       <c r="C146" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D146" t="s">
         <v>165</v>
@@ -4748,10 +4974,10 @@
         <v>145</v>
       </c>
       <c r="C147" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D147" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
@@ -4759,10 +4985,10 @@
         <v>133</v>
       </c>
       <c r="C148" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D148" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
@@ -4770,7 +4996,7 @@
         <v>55</v>
       </c>
       <c r="C149" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D149" t="s">
         <v>165</v>
@@ -4781,7 +5007,7 @@
         <v>56</v>
       </c>
       <c r="C150" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D150" t="s">
         <v>165</v>
@@ -4792,7 +5018,7 @@
         <v>57</v>
       </c>
       <c r="C151" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D151" t="s">
         <v>165</v>
@@ -4803,7 +5029,7 @@
         <v>134</v>
       </c>
       <c r="C152" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D152" t="s">
         <v>166</v>
@@ -4814,10 +5040,10 @@
         <v>150</v>
       </c>
       <c r="C153" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D153" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
@@ -4825,7 +5051,7 @@
         <v>135</v>
       </c>
       <c r="C154" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D154" t="s">
         <v>165</v>
@@ -4836,7 +5062,7 @@
         <v>127</v>
       </c>
       <c r="C155" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D155" t="s">
         <v>165</v>
@@ -4847,7 +5073,7 @@
         <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D156" t="s">
         <v>165</v>
@@ -4858,7 +5084,7 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D157" t="s">
         <v>165</v>
@@ -4869,14 +5095,19 @@
         <v>113</v>
       </c>
       <c r="C158" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D158" t="s">
         <v>165</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:D158" xr:uid="{020EC039-F7E7-4DEF-AE9A-E6C4DE324E37}"/>
+  <autoFilter ref="B2:D158" xr:uid="{020EC039-F7E7-4DEF-AE9A-E6C4DE324E37}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D158">
+      <sortCondition ref="C2:C158"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>